<commit_message>
Cleaned bugs, adjusted Code to randomly allocate people with flexible time preference to either week to make sure that people with specific week availability are not discriminated.
</commit_message>
<xml_diff>
--- a/Rankings.xlsx
+++ b/Rankings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschl\OneDrive\Documents\Klimadelegation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jschl\OneDrive\Documents\Klimadelegation\COP26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336A38E1-5EFF-4D2A-B355-EA18BB1CB126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64722671-9F74-46FF-B059-36758F3A4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F4ECAC2-64DE-4C39-AD9D-977EF7138168}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Hannah</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
     <t>Peter</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>nein</t>
+  </si>
+  <si>
+    <t>nm</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -475,16 +475,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
       <c r="E2">
         <v>7</v>
@@ -492,16 +492,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -509,16 +509,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>9</v>
@@ -526,16 +526,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -543,16 +543,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
       </c>
       <c r="E6">
         <v>9</v>
@@ -560,16 +560,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -577,16 +577,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -600,10 +600,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -611,16 +611,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -628,16 +628,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -645,16 +645,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>10</v>

</xml_diff>